<commit_message>
update SMARTS data dictionaries
</commit_message>
<xml_diff>
--- a/SMARTS/Data_Dictionaries/Stormwater_Construction_Monitoring_DataDictionary.xlsx
+++ b/SMARTS/Data_Dictionaries/Stormwater_Construction_Monitoring_DataDictionary.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawaterboards-my.sharepoint.com/personal/david_altare_waterboards_ca_gov/Documents/projects/CA_data_portal/SMARTS/Data_Dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{F2563C35-6E67-4285-AEDE-D8B0C195017C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7688DD2D-3571-4D30-B60F-9028985DE6EE}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{F2563C35-6E67-4285-AEDE-D8B0C195017C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C141CB62-516A-491A-85B3-E7B4CB616D2C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DA1BC090-5ABE-44CD-AF01-7218500D7CAD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Industrial_Facilities" sheetId="1" r:id="rId1"/>
+    <sheet name="Construction_Monitoring" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="84">
-  <si>
-    <t>Regulatory Measure Type (Permit Type)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="94">
   <si>
     <t>PERMIT_TYPE</t>
   </si>
@@ -44,24 +41,12 @@
     <t>Type of permit or application.</t>
   </si>
   <si>
-    <t>Regulatory Measure ID (Application ID)</t>
-  </si>
-  <si>
     <t>APP_ID</t>
   </si>
   <si>
-    <t>A unique Identification number associated with a storm water application.  Universal number used to link the application to inspections, violations, and enforcement actions.</t>
-  </si>
-  <si>
-    <t>Waste Discharge ID</t>
-  </si>
-  <si>
     <t>WDID</t>
   </si>
   <si>
-    <t xml:space="preserve">Identification number associated with a waste discharge. </t>
-  </si>
-  <si>
     <t>column</t>
   </si>
   <si>
@@ -86,12 +71,6 @@
     <t>Reporting Year</t>
   </si>
   <si>
-    <t>Reporting year the sample was collected in.</t>
-  </si>
-  <si>
-    <t>Report ID</t>
-  </si>
-  <si>
     <t>REPORT_ID</t>
   </si>
   <si>
@@ -101,48 +80,30 @@
     <t>MONITORING_LOCATION_NAME</t>
   </si>
   <si>
-    <t>Name of the monitoring location at the regulated facility/site.</t>
-  </si>
-  <si>
     <t>Monitoring Location Type</t>
   </si>
   <si>
     <t>MONITORING_LOCATION_TYPE</t>
   </si>
   <si>
-    <t>Type of monitoring location at the regulated facility/site.</t>
-  </si>
-  <si>
     <t>Monitoring Location Description</t>
   </si>
   <si>
     <t>MONITOR_LOCATION_DESCRIPTION</t>
   </si>
   <si>
-    <t>Description of the monitoring location at the regulated facility/site.</t>
-  </si>
-  <si>
     <t>Monitoring Location Latitude</t>
   </si>
   <si>
     <t>MONITORING_LATITUDE</t>
   </si>
   <si>
-    <t>Latitude used to map the regulated facility/site monitoring location, expressed in decimal degrees.</t>
-  </si>
-  <si>
     <t>Monitoring Location Longitude</t>
   </si>
   <si>
     <t>MONITORING_LONGITUDE</t>
   </si>
   <si>
-    <t>Longitude used to map the regulated facility/site monitoring location, expressed in decimal degrees.</t>
-  </si>
-  <si>
-    <t>Sample ID Number</t>
-  </si>
-  <si>
     <t>SAMPLE_ID</t>
   </si>
   <si>
@@ -152,18 +113,12 @@
     <t>SAMPLE_DATE</t>
   </si>
   <si>
-    <t>Date the sample was collected a storm event at a specific monitoring location.</t>
-  </si>
-  <si>
     <t>Sample Time</t>
   </si>
   <si>
     <t>SAMPLE_TIME</t>
   </si>
   <si>
-    <t>Time the sample was collected a storm event at a specific monitoring location.</t>
-  </si>
-  <si>
     <t>Parameter</t>
   </si>
   <si>
@@ -197,9 +152,6 @@
     <t>Analytical Method</t>
   </si>
   <si>
-    <t>Analytical test method performed.</t>
-  </si>
-  <si>
     <t>Method Detection Limit</t>
   </si>
   <si>
@@ -275,13 +227,7 @@
     <t>Rainfall Amount</t>
   </si>
   <si>
-    <t xml:space="preserve">The measurement used to address the level of a parameter. </t>
-  </si>
-  <si>
     <t>Identification number associated with the sample.</t>
-  </si>
-  <si>
-    <t>Identification number associated with the report.</t>
   </si>
   <si>
     <t>Reported analytical result qualifier:
@@ -290,6 +236,90 @@
 - "=": Equal to
 - "&gt;": Greater than
 - "&lt;": Less than</t>
+  </si>
+  <si>
+    <t>Permit Type</t>
+  </si>
+  <si>
+    <t>Waste Discharge Identification Number</t>
+  </si>
+  <si>
+    <t>Unique identification number assigned to the discharger for a specified facility.</t>
+  </si>
+  <si>
+    <t>Application Identification Number</t>
+  </si>
+  <si>
+    <t>Unique identification number associated with a storm water application, used to link the application to inspections, violations, and enforcement actions.</t>
+  </si>
+  <si>
+    <t>Reporting period that the sample was collected in (reporting period is July 1-June 30).</t>
+  </si>
+  <si>
+    <t>Report Identification Number</t>
+  </si>
+  <si>
+    <t>Unique identification number associated with the report.</t>
+  </si>
+  <si>
+    <t>Type of event (e.g., qualifying storm event, non-qualifying storm event, non-stormwater discharge).</t>
+  </si>
+  <si>
+    <t>The date the storm event started at the site.</t>
+  </si>
+  <si>
+    <t>The date the storm event ended at the site.</t>
+  </si>
+  <si>
+    <t>Amount of rainfall at the site during the storm event.</t>
+  </si>
+  <si>
+    <t>Name of the monitoring location at the regulated site.</t>
+  </si>
+  <si>
+    <t>Type of monitoring location at the regulated site.</t>
+  </si>
+  <si>
+    <t>Description of the monitoring location at the regulated site.</t>
+  </si>
+  <si>
+    <t>Latitude used to map the monitoring location at the regulated site, expressed in decimal degrees.</t>
+  </si>
+  <si>
+    <t>Longitude used to map the monitoring location at the regulated site, expressed in decimal degrees.</t>
+  </si>
+  <si>
+    <t>Sample Identification Number</t>
+  </si>
+  <si>
+    <t>Date the sample was collected.</t>
+  </si>
+  <si>
+    <t>Time the sample was collected.</t>
+  </si>
+  <si>
+    <t>Qualified SWPPP Practitioner (QSP) Name</t>
+  </si>
+  <si>
+    <t>Name of the Qualified Stormwater Pollution Prevention Plan (SWPPP) Practitioner (QSP).</t>
+  </si>
+  <si>
+    <t>The unit of measurement for the result (e.g., mg/L, ug/L, etc.).</t>
+  </si>
+  <si>
+    <t>Analytical test method used for the sample.</t>
+  </si>
+  <si>
+    <t>Name of individual who certified the reported data.</t>
+  </si>
+  <si>
+    <t>Date the reported data was certified.</t>
+  </si>
+  <si>
+    <t>Analyzed By</t>
+  </si>
+  <si>
+    <t>Name of individual who analyzed the sample.</t>
   </si>
 </sst>
 </file>
@@ -320,12 +350,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="4">
@@ -383,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -399,6 +435,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -751,9 +790,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EC05117-1A42-4E74-BDC4-6F8548E0C8AB}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,97 +805,97 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>8</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>69</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>72</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>74</v>
@@ -864,338 +903,338 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>72</v>
+        <v>49</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>74</v>
+        <v>9</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>73</v>
+        <v>50</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>74</v>
+        <v>9</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>79</v>
+        <v>51</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>74</v>
+        <v>10</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>74</v>
+        <v>52</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>74</v>
+        <v>10</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>25</v>
+        <v>79</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>28</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>31</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>34</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>35</v>
+        <v>83</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>74</v>
+        <v>54</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>86</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>74</v>
+        <v>8</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>83</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>74</v>
+        <v>55</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>74</v>
+        <v>8</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>76</v>
+        <v>59</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>60</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>74</v>
+        <v>8</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>61</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>74</v>
+        <v>8</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>